<commit_message>
#17 Added API routes POST /publishers, GET /publishers, GET /publishers/{id}, and PUT /publishers/{id}.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A58A7B36-E1D8-4B61-9E1D-8E091659BCD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062C3296-B352-4D74-8053-FDA113B78035}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24015" yWindow="-20910" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
+    <workbookView xWindow="4200" yWindow="-17355" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
   <si>
     <t>Verb</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>/users/{user-id}/accounts/{user-account-id}</t>
+  </si>
+  <si>
+    <t>/users/{user-id}/login</t>
   </si>
 </sst>
 </file>
@@ -145,15 +148,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -161,12 +170,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E85610-9C68-46E3-9E1F-93752A63B169}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +530,7 @@
     <col min="2" max="2" width="82.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,341 +538,392 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>10</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>2</v>
       </c>
       <c r="B26" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>10</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>7</v>
       </c>
       <c r="B28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>2</v>
       </c>
       <c r="B29" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>22</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>7</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>2</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>22</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>7</v>
       </c>
       <c r="B34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>2</v>
       </c>
       <c r="B35" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
       <c r="B36" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>7</v>
       </c>
       <c r="B37" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>2</v>
       </c>
       <c r="B38" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>2</v>
       </c>
       <c r="B39" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>10</v>
       </c>
       <c r="B40" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>7</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>2</v>
       </c>
       <c r="B42" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>22</v>
       </c>
       <c r="B43" t="s">
         <v>31</v>
       </c>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#17 Added API routes POST /artists, GET /artists, GET /artists/{id}, and PUT /artists/{id}.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062C3296-B352-4D74-8053-FDA113B78035}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E3A404-A706-42BD-BD64-2EDC3FE0AB6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="-17355" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
+    <workbookView xWindow="25650" yWindow="-17160" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Routes" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
-  <si>
-    <t>Verb</t>
-  </si>
-  <si>
-    <t>Route</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="31">
   <si>
     <t>GET</t>
   </si>
@@ -162,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -170,29 +164,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,17 +188,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{41B12572-AEAA-4D3B-9A48-28464028844B}" name="Table3" displayName="Table3" ref="A1:B1048576" totalsRowShown="0">
-  <autoFilter ref="A1:B1048576" xr:uid="{65AB9418-F346-4C60-9AF7-E5C31C682BDD}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{34AA3EDB-23A3-4571-B6F9-EE2E550C7999}" name="Verb"/>
-    <tableColumn id="2" xr3:uid="{EE5395AA-8552-4C59-9C49-D3661446E633}" name="Route"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,418 +486,422 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E85610-9C68-46E3-9E1F-93752A63B169}">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
+  <dimension ref="A2:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" customWidth="1"/>
-    <col min="2" max="2" width="82.81640625" customWidth="1"/>
+    <col min="1" max="1" width="3.07421875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.61328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.61328125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B36" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" t="s">
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="2"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#17 Added API routes POST /, POST /users, GET /users, GET /users/{id}, and PUT /users/{id}, POST /login.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E3A404-A706-42BD-BD64-2EDC3FE0AB6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1F9AD6-D606-4716-BC7B-CDD2C769375F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25650" yWindow="-17160" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
   <si>
     <t>GET</t>
   </si>
@@ -126,7 +126,10 @@
     <t>/users/{user-id}/accounts/{user-account-id}</t>
   </si>
   <si>
-    <t>/users/{user-id}/login</t>
+    <t>/users?type={type-id}</t>
+  </si>
+  <si>
+    <t>/login</t>
   </si>
 </sst>
 </file>
@@ -489,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
   <dimension ref="A2:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -674,6 +677,7 @@
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
@@ -682,6 +686,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,6 +695,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" s="3"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,6 +704,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
@@ -745,7 +752,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
@@ -753,7 +760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
@@ -761,7 +768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B36" s="1" t="s">
         <v>20</v>
       </c>
@@ -777,7 +784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
@@ -785,7 +792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B38" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,7 +800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B39" s="1" t="s">
         <v>20</v>
       </c>
@@ -801,11 +808,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B41" s="1" t="s">
         <v>5</v>
       </c>
@@ -813,7 +820,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B42" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,7 +828,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B43" s="1" t="s">
         <v>8</v>
       </c>
@@ -829,11 +836,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" s="3"/>
       <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
@@ -841,15 +849,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" s="3"/>
       <c r="B46" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" s="3"/>
       <c r="B47" s="1" t="s">
         <v>0</v>
       </c>
@@ -857,7 +867,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" s="3"/>
       <c r="B48" s="1" t="s">
         <v>8</v>
       </c>
@@ -865,15 +876,16 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49" s="3"/>
       <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
@@ -881,7 +893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B51" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +901,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B52" s="1" t="s">
         <v>20</v>
       </c>
@@ -897,7 +909,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>

</xml_diff>

<commit_message>
#17 Added API routes POST /users/{user-id}/accounts, GET /users/{user-id}/accounts, PUT /users/{user-id}/accounts/{user-account-id}, and DELETE /users/{user-id}/accounts/{user-account-id}.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1F9AD6-D606-4716-BC7B-CDD2C769375F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED224D0-5FB3-4E21-A540-448879437F37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25650" yWindow="-17160" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
   <si>
     <t>GET</t>
   </si>
@@ -171,11 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
-  <dimension ref="A2:C53"/>
+  <dimension ref="A2:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -505,6 +506,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -886,6 +888,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
@@ -894,6 +897,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51" s="3"/>
       <c r="B51" s="1" t="s">
         <v>0</v>
       </c>
@@ -902,16 +906,26 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B52" s="1" t="s">
-        <v>20</v>
+      <c r="A52" s="3"/>
+      <c r="B52" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#17 Added API routes POST /users/{user-id}/links, GET /users/{user-id}/links, and DELETE /users/{user-id}/links/{user-link-id}.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED224D0-5FB3-4E21-A540-448879437F37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16C68C5-6FFE-4434-AD1C-122041BC8FCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25650" yWindow="-17160" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
+    <workbookView xWindow="27480" yWindow="-18495" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>GET</t>
   </si>
@@ -130,6 +130,126 @@
   </si>
   <si>
     <t>/login</t>
+  </si>
+  <si>
+    <t>Seed database</t>
+  </si>
+  <si>
+    <t>Get installation</t>
+  </si>
+  <si>
+    <t>List countries</t>
+  </si>
+  <si>
+    <t>List services</t>
+  </si>
+  <si>
+    <t>List performing rights organiations</t>
+  </si>
+  <si>
+    <t>List platforms</t>
+  </si>
+  <si>
+    <t>Add platform</t>
+  </si>
+  <si>
+    <t>Get platform</t>
+  </si>
+  <si>
+    <t>Update platform</t>
+  </si>
+  <si>
+    <t>Add publisher</t>
+  </si>
+  <si>
+    <t>List publishers</t>
+  </si>
+  <si>
+    <t>Get publisher</t>
+  </si>
+  <si>
+    <t>Update publisher</t>
+  </si>
+  <si>
+    <t>Add record label</t>
+  </si>
+  <si>
+    <t>List record labels</t>
+  </si>
+  <si>
+    <t>Get record label</t>
+  </si>
+  <si>
+    <t>Update record label</t>
+  </si>
+  <si>
+    <t>List artists</t>
+  </si>
+  <si>
+    <t>Add artist</t>
+  </si>
+  <si>
+    <t>Get artist</t>
+  </si>
+  <si>
+    <t>Update artist</t>
+  </si>
+  <si>
+    <t>Add user</t>
+  </si>
+  <si>
+    <t>List users</t>
+  </si>
+  <si>
+    <t>Get user</t>
+  </si>
+  <si>
+    <t>Update user</t>
+  </si>
+  <si>
+    <t>Login user</t>
+  </si>
+  <si>
+    <t>Add user account</t>
+  </si>
+  <si>
+    <t>List user accounts</t>
+  </si>
+  <si>
+    <t>Remove user account</t>
+  </si>
+  <si>
+    <t>Update user account</t>
+  </si>
+  <si>
+    <t>Send user invitation</t>
+  </si>
+  <si>
+    <t>Get user invitation</t>
+  </si>
+  <si>
+    <t>Accept user invitation</t>
+  </si>
+  <si>
+    <t>List artist accounts</t>
+  </si>
+  <si>
+    <t>List artist links</t>
+  </si>
+  <si>
+    <t>Update artist account</t>
+  </si>
+  <si>
+    <t>Remove artist account</t>
+  </si>
+  <si>
+    <t>Add artist account</t>
+  </si>
+  <si>
+    <t>Add artist link</t>
+  </si>
+  <si>
+    <t>Remove artist link</t>
   </si>
 </sst>
 </file>
@@ -171,12 +291,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
-  <dimension ref="A2:C54"/>
+  <dimension ref="A2:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -502,10 +623,11 @@
     <col min="1" max="1" width="3.07421875" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.61328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="45.61328125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.23046875" style="2"/>
+    <col min="4" max="4" width="33.3046875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -513,8 +635,11 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -522,12 +647,15 @@
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -535,8 +663,11 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -544,8 +675,11 @@
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D6" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>0</v>
@@ -553,12 +687,15 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -566,8 +703,11 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -575,8 +715,11 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D10" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>0</v>
@@ -584,8 +727,11 @@
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D11" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -593,12 +739,15 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D12" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -606,8 +755,11 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>0</v>
@@ -615,8 +767,11 @@
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D15" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>0</v>
@@ -624,8 +779,11 @@
       <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D16" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
         <v>8</v>
@@ -633,12 +791,15 @@
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D17" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>5</v>
@@ -646,8 +807,11 @@
       <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D19" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="1" t="s">
         <v>0</v>
@@ -655,8 +819,11 @@
       <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D20" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
         <v>0</v>
@@ -664,8 +831,11 @@
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D21" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -673,12 +843,15 @@
       <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D22" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
         <v>5</v>
@@ -686,8 +859,11 @@
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D24" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>0</v>
@@ -695,8 +871,11 @@
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D25" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -704,8 +883,11 @@
       <c r="C26" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D26" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
         <v>8</v>
@@ -713,8 +895,11 @@
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D27" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
@@ -722,7 +907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
@@ -738,7 +923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
@@ -746,7 +931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,7 +939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
@@ -762,170 +947,242 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" s="3"/>
       <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D34" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A35" s="3"/>
       <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B36" s="1" t="s">
-        <v>20</v>
+      <c r="D35" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D36" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" s="3"/>
       <c r="B37" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="3"/>
       <c r="B38" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D38" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" s="3"/>
       <c r="B39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" s="3"/>
+      <c r="B40" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="D40" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D42" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B43" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" s="3"/>
-      <c r="B45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D43" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46" s="3"/>
       <c r="B46" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47" s="3"/>
       <c r="B47" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48" s="3"/>
       <c r="B48" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D48" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" s="3"/>
       <c r="B49" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51" s="3"/>
       <c r="B51" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D51" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" s="3"/>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A53" s="3"/>
+      <c r="B53" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" s="3"/>
-      <c r="B53" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="D53" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A54" s="3"/>
+      <c r="B54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#17 Added localization framework and token replacement service. Added en-US resources and task base class.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16C68C5-6FFE-4434-AD1C-122041BC8FCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A949E153-A27B-4D6A-86BA-3811579C8EF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27480" yWindow="-18495" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
+    <workbookView xWindow="26670" yWindow="-16755" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
   <si>
     <t>GET</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>Remove artist link</t>
+  </si>
+  <si>
+    <t>Add artist member</t>
+  </si>
+  <si>
+    <t>List artist members</t>
+  </si>
+  <si>
+    <t>Update artist member</t>
   </si>
 </sst>
 </file>
@@ -614,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
   <dimension ref="A2:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -900,30 +909,43 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" s="3"/>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D28" s="5" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" s="3"/>
       <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D29" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" s="3"/>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D30" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" s="3"/>
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
@@ -932,6 +954,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" s="3"/>
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
@@ -940,6 +963,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" s="3"/>
       <c r="B33" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
#17 Added API routes POST /invitations, GET /invitations/{uuid}, and POST /invitations/{uuid}.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A949E153-A27B-4D6A-86BA-3811579C8EF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967B6F1A-A241-4B25-821D-F0ED22C02224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26670" yWindow="-16755" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
+    <workbookView xWindow="26235" yWindow="-16875" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="2" r:id="rId1"/>
@@ -623,9 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
   <dimension ref="A2:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1060,6 +1058,7 @@
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" s="3"/>
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1071,6 +1070,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A43" s="3"/>
       <c r="B43" s="1" t="s">
         <v>0</v>
       </c>
@@ -1082,6 +1082,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" s="3"/>
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
#23 Added security requirements to Api Endpoints.xlsx
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967B6F1A-A241-4B25-821D-F0ED22C02224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1726AAEC-0830-4ECB-8AFD-0C09EDED54D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26235" yWindow="-16875" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
+    <workbookView xWindow="22470" yWindow="-20055" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
   <si>
     <t>GET</t>
   </si>
@@ -259,6 +259,39 @@
   </si>
   <si>
     <t>Update artist member</t>
+  </si>
+  <si>
+    <t>Anon</t>
+  </si>
+  <si>
+    <t>SysAdmin</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>SysAdmin, PublisherAdmin</t>
+  </si>
+  <si>
+    <t>SysAdmin, LabelAdmin</t>
+  </si>
+  <si>
+    <t>SysAdmin, LabelAdmin, ArtistMember, ArtistManager</t>
+  </si>
+  <si>
+    <t>Add artist manager</t>
+  </si>
+  <si>
+    <t>Update artist manager</t>
+  </si>
+  <si>
+    <t>List artist managers</t>
+  </si>
+  <si>
+    <t>SysAdmin, LabelAdmin, PubAdmin</t>
+  </si>
+  <si>
+    <t>SysAdmin, LabelAdmin, PubAdmin, Self</t>
   </si>
 </sst>
 </file>
@@ -621,9 +654,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
-  <dimension ref="A2:D55"/>
+  <dimension ref="A2:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -631,10 +666,11 @@
     <col min="2" max="2" width="9.61328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="45.61328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="33.3046875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.23046875" style="2"/>
+    <col min="5" max="5" width="51.69140625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -645,8 +681,11 @@
       <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E2" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -657,12 +696,15 @@
       <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E3" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>0</v>
@@ -673,8 +715,11 @@
       <c r="D5" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E5" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -685,8 +730,11 @@
       <c r="D6" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E6" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>0</v>
@@ -697,12 +745,15 @@
       <c r="D7" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E7" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -714,7 +765,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -726,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>0</v>
@@ -738,7 +789,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -750,11 +801,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -765,8 +816,11 @@
       <c r="D14" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E14" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>0</v>
@@ -777,8 +831,11 @@
       <c r="D15" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E15" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>0</v>
@@ -789,8 +846,11 @@
       <c r="D16" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E16" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
         <v>8</v>
@@ -801,12 +861,15 @@
       <c r="D17" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E17" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>5</v>
@@ -817,8 +880,11 @@
       <c r="D19" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E19" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="1" t="s">
         <v>0</v>
@@ -829,8 +895,11 @@
       <c r="D20" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E20" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
         <v>0</v>
@@ -841,8 +910,11 @@
       <c r="D21" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E21" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -853,12 +925,15 @@
       <c r="D22" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E22" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
         <v>5</v>
@@ -869,8 +944,11 @@
       <c r="D24" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E24" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>0</v>
@@ -881,8 +959,11 @@
       <c r="D25" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E25" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -893,8 +974,11 @@
       <c r="D26" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E26" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
         <v>8</v>
@@ -905,8 +989,11 @@
       <c r="D27" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E27" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="1" t="s">
         <v>5</v>
@@ -917,8 +1004,11 @@
       <c r="D28" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E28" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="3"/>
       <c r="B29" s="1" t="s">
         <v>0</v>
@@ -929,8 +1019,11 @@
       <c r="D29" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E29" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="B30" s="1" t="s">
         <v>8</v>
@@ -941,8 +1034,11 @@
       <c r="D30" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E30" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="3"/>
       <c r="B31" s="1" t="s">
         <v>5</v>
@@ -950,8 +1046,14 @@
       <c r="C31" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D31" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="3"/>
       <c r="B32" s="1" t="s">
         <v>0</v>
@@ -959,8 +1061,14 @@
       <c r="C32" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D32" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="3"/>
       <c r="B33" s="1" t="s">
         <v>8</v>
@@ -968,8 +1076,14 @@
       <c r="C33" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D33" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="3"/>
       <c r="B34" s="1" t="s">
         <v>5</v>
@@ -980,8 +1094,11 @@
       <c r="D34" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E34" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="3"/>
       <c r="B35" s="1" t="s">
         <v>0</v>
@@ -992,8 +1109,11 @@
       <c r="D35" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E35" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>8</v>
@@ -1004,8 +1124,11 @@
       <c r="D36" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E36" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
       <c r="B37" s="1" t="s">
         <v>20</v>
@@ -1016,8 +1139,11 @@
       <c r="D37" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E37" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="3"/>
       <c r="B38" s="1" t="s">
         <v>5</v>
@@ -1028,8 +1154,11 @@
       <c r="D38" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E38" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="3"/>
       <c r="B39" s="1" t="s">
         <v>0</v>
@@ -1040,8 +1169,11 @@
       <c r="D39" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E39" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="3"/>
       <c r="B40" s="1" t="s">
         <v>20</v>
@@ -1052,12 +1184,15 @@
       <c r="D40" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E40" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="3"/>
       <c r="B42" s="1" t="s">
         <v>5</v>
@@ -1068,8 +1203,11 @@
       <c r="D42" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E42" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" s="3"/>
       <c r="B43" s="1" t="s">
         <v>0</v>
@@ -1080,8 +1218,11 @@
       <c r="D43" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E43" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="3"/>
       <c r="B44" s="1" t="s">
         <v>5</v>
@@ -1092,12 +1233,15 @@
       <c r="D44" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E44" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" s="3"/>
       <c r="B46" s="1" t="s">
         <v>5</v>
@@ -1108,8 +1252,11 @@
       <c r="D46" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E46" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="3"/>
       <c r="B47" s="1" t="s">
         <v>0</v>
@@ -1120,8 +1267,11 @@
       <c r="D47" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E47" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" s="3"/>
       <c r="B48" s="1" t="s">
         <v>0</v>
@@ -1132,8 +1282,11 @@
       <c r="D48" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E48" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" s="3"/>
       <c r="B49" s="1" t="s">
         <v>8</v>
@@ -1144,8 +1297,11 @@
       <c r="D49" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E49" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
         <v>5</v>
@@ -1156,8 +1312,11 @@
       <c r="D50" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E50" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="3"/>
       <c r="B51" s="1" t="s">
         <v>5</v>
@@ -1168,8 +1327,11 @@
       <c r="D51" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E51" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="3"/>
       <c r="B52" s="1" t="s">
         <v>0</v>
@@ -1180,8 +1342,11 @@
       <c r="D52" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E52" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" s="3"/>
       <c r="B53" s="4" t="s">
         <v>8</v>
@@ -1192,8 +1357,11 @@
       <c r="D53" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E53" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" s="3"/>
       <c r="B54" s="1" t="s">
         <v>20</v>
@@ -1204,8 +1372,11 @@
       <c r="D54" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E54" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>

</xml_diff>

<commit_message>
#23 Added API authentication and data redaction based on user roles and relationships.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1726AAEC-0830-4ECB-8AFD-0C09EDED54D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B703CE46-F69E-4382-ABA3-5A96985BF07F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22470" yWindow="-20055" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
+    <workbookView xWindow="25920" yWindow="-18945" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="2" r:id="rId1"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="88">
   <si>
     <t>GET</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>/countries</t>
   </si>
   <si>
@@ -270,15 +267,6 @@
     <t>Any</t>
   </si>
   <si>
-    <t>SysAdmin, PublisherAdmin</t>
-  </si>
-  <si>
-    <t>SysAdmin, LabelAdmin</t>
-  </si>
-  <si>
-    <t>SysAdmin, LabelAdmin, ArtistMember, ArtistManager</t>
-  </si>
-  <si>
     <t>Add artist manager</t>
   </si>
   <si>
@@ -291,15 +279,127 @@
     <t>SysAdmin, LabelAdmin, PubAdmin</t>
   </si>
   <si>
-    <t>SysAdmin, LabelAdmin, PubAdmin, Self</t>
+    <t>/system</t>
+  </si>
+  <si>
+    <t>/system/seed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SysAdmin, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PublisherAdmin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SysAdmin, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LabelAdmin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SysAdmin, LabelAdmin, PubAdmin, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SysUser</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SysAdmin, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LabelAdmin, SysUser</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SysAdmin, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LabelAdmin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SysUser</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -656,9 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
   <dimension ref="A2:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -673,31 +771,31 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -710,13 +808,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -725,13 +823,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -740,13 +838,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
@@ -756,13 +854,16 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
@@ -771,10 +872,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
@@ -783,22 +887,28 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
@@ -808,16 +918,16 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
@@ -826,13 +936,13 @@
         <v>0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
@@ -841,28 +951,28 @@
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
@@ -872,16 +982,16 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
@@ -890,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -905,28 +1015,28 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
@@ -936,16 +1046,16 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
@@ -954,13 +1064,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
@@ -969,43 +1079,43 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
@@ -1014,43 +1124,43 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="B30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="3"/>
       <c r="B31" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
@@ -1059,43 +1169,43 @@
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="3"/>
       <c r="B33" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="3"/>
       <c r="B34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
@@ -1104,58 +1214,58 @@
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
       <c r="B37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D37" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="3"/>
       <c r="B38" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
@@ -1164,28 +1274,28 @@
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="3"/>
       <c r="B40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
@@ -1195,16 +1305,16 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="3"/>
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
@@ -1213,28 +1323,28 @@
         <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="3"/>
       <c r="B44" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.4">
@@ -1244,31 +1354,31 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" s="3"/>
       <c r="B46" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>53</v>
+        <v>30</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="3"/>
       <c r="B47" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
@@ -1277,25 +1387,25 @@
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" s="3"/>
       <c r="B49" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>56</v>
+        <v>26</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>85</v>
@@ -1304,28 +1414,28 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="3"/>
       <c r="B51" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>85</v>
@@ -1337,10 +1447,10 @@
         <v>0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>85</v>
@@ -1349,13 +1459,13 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" s="3"/>
       <c r="B53" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>85</v>
@@ -1364,13 +1474,13 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" s="3"/>
       <c r="B54" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>85</v>
@@ -1382,5 +1492,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#23 Updated endpoint spreadsheet. Changed access rules on list artist links.
</commit_message>
<xml_diff>
--- a/Server/Documentation/Api Endpoints.xlsx
+++ b/Server/Documentation/Api Endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Songtracker Pro\Code\Server\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B703CE46-F69E-4382-ABA3-5A96985BF07F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D20DA7-E3B9-4FAA-976F-4AE5F4AA6B05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25920" yWindow="-18945" windowWidth="22905" windowHeight="16095" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
+    <workbookView xWindow="1509" yWindow="1509" windowWidth="18514" windowHeight="10834" xr2:uid="{A88B1A8D-B508-4007-B141-8904DC78A6DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="2" r:id="rId1"/>
@@ -756,7 +756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2325BC09-A649-40E1-B795-67178C4F96F5}">
   <dimension ref="A2:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1280,7 +1282,7 @@
         <v>65</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">

</xml_diff>